<commit_message>
feat(user-management): enhance CRUD flows, stabilize page objects, and expand tests
- Update pages `pages/userManagement.page.ts` and `pages/userManagementNewUser.page.ts` to refine locators and improve reliability for create/update/delete flows
- Extend E2E coverage in `tests/web/UserManagement/1. UserCreateUpdateDeleteTest.spec.ts`
- Refresh test data: update `test_data/UserManagementTestData/user_update.csv` and Excel report
- Add new artifacts: `test_data/UserManagementTestData/ExportData/` and `test_data/UserManagementTestData/userSearchTestData.json`
- Tweak environment handling in `utils/env.ts`
- Improve role management scenarios in:
  - `tests/web/RoleManagement/1. TestShadowRole.spec.ts`
  - `tests/web/RoleManagement/2.TestManagerRole.spec.ts`

Refs: userManagementTest
</commit_message>
<xml_diff>
--- a/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
+++ b/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
@@ -429,7 +429,7 @@
         <v>test.bulk.user1@brainstation-23.com</v>
       </c>
       <c r="D2" t="str">
-        <v>e3e6460f-9b05-4016-8d7d-e77f17649b2b</v>
+        <v>8f2d0c08-f7ad-4935-a6e5-c52dde1be5e0</v>
       </c>
     </row>
     <row r="3">
@@ -443,7 +443,7 @@
         <v>test.bulk.user2@brainstation-23.com</v>
       </c>
       <c r="D3" t="str">
-        <v>c3e85d52-b85e-4da3-8e8c-162d2526e132</v>
+        <v>1d2c95f6-a889-49b9-9bcc-3908c7ca40c1</v>
       </c>
     </row>
     <row r="4">
@@ -457,7 +457,7 @@
         <v>test.bulk.user3@brainstation-23.com</v>
       </c>
       <c r="D4" t="str">
-        <v>a43b47ff-509a-4721-bf68-85a2f1d8f79c</v>
+        <v>7b0f8a3b-b7a0-4b9f-a880-a945f60ee21e</v>
       </c>
     </row>
     <row r="5">
@@ -471,7 +471,7 @@
         <v>test.bulk.user4@brainstation-23.com</v>
       </c>
       <c r="D5" t="str">
-        <v>cd285b2b-3aaf-4fed-a23d-2dcdf7e27aba</v>
+        <v>fd395b8e-1bbb-4a51-829b-27a6beb7f4f3</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>Report Generated</v>
       </c>
       <c r="B6" t="str">
-        <v>10/27/2025, 1:54:19 PM</v>
+        <v>10/28/2025, 8:17:23 PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add test tagging and GitHub Actions CI workflow
- Add @user-management tags to UserManagement test suite
- Implement GitHub Actions workflow for Playwright test automation
  - Manual trigger with environment selection
  - Automated artifact upload and dependency caching
</commit_message>
<xml_diff>
--- a/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
+++ b/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
@@ -429,7 +429,7 @@
         <v>test.bulk.user1@brainstation-23.com</v>
       </c>
       <c r="D2" t="str">
-        <v>8f2d0c08-f7ad-4935-a6e5-c52dde1be5e0</v>
+        <v>2e1afb38-45a5-41ae-9b63-9ab2c2c755cb</v>
       </c>
     </row>
     <row r="3">
@@ -443,7 +443,7 @@
         <v>test.bulk.user2@brainstation-23.com</v>
       </c>
       <c r="D3" t="str">
-        <v>1d2c95f6-a889-49b9-9bcc-3908c7ca40c1</v>
+        <v>a760c524-bdb6-4454-9939-02e59dd7031d</v>
       </c>
     </row>
     <row r="4">
@@ -457,7 +457,7 @@
         <v>test.bulk.user3@brainstation-23.com</v>
       </c>
       <c r="D4" t="str">
-        <v>7b0f8a3b-b7a0-4b9f-a880-a945f60ee21e</v>
+        <v>051fc0a9-91fc-4865-84ed-d48d92026fb3</v>
       </c>
     </row>
     <row r="5">
@@ -471,7 +471,7 @@
         <v>test.bulk.user4@brainstation-23.com</v>
       </c>
       <c r="D5" t="str">
-        <v>fd395b8e-1bbb-4a51-829b-27a6beb7f4f3</v>
+        <v>e522f464-167a-47f9-af6b-5de82126ad80</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>Report Generated</v>
       </c>
       <c r="B6" t="str">
-        <v>10/28/2025, 8:17:23 PM</v>
+        <v>11/10/2025, 3:18:26 PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update and delete user information
</commit_message>
<xml_diff>
--- a/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
+++ b/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
@@ -429,7 +429,7 @@
         <v>test.bulk.user1@brainstation-23.com</v>
       </c>
       <c r="D2" t="str">
-        <v>2e1afb38-45a5-41ae-9b63-9ab2c2c755cb</v>
+        <v>0b4b62a1-3e91-45cf-94ac-fb94a84ef9a4</v>
       </c>
     </row>
     <row r="3">
@@ -443,7 +443,7 @@
         <v>test.bulk.user2@brainstation-23.com</v>
       </c>
       <c r="D3" t="str">
-        <v>a760c524-bdb6-4454-9939-02e59dd7031d</v>
+        <v>984b1f58-9233-4ec0-a193-30417b5ac9bd</v>
       </c>
     </row>
     <row r="4">
@@ -457,7 +457,7 @@
         <v>test.bulk.user3@brainstation-23.com</v>
       </c>
       <c r="D4" t="str">
-        <v>051fc0a9-91fc-4865-84ed-d48d92026fb3</v>
+        <v>23ed4a6a-2467-48e5-a217-bf69106e9463</v>
       </c>
     </row>
     <row r="5">
@@ -471,7 +471,7 @@
         <v>test.bulk.user4@brainstation-23.com</v>
       </c>
       <c r="D5" t="str">
-        <v>e522f464-167a-47f9-af6b-5de82126ad80</v>
+        <v>e8fc1a8e-bb04-421c-9fda-a519919c51b9</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>Report Generated</v>
       </c>
       <c r="B6" t="str">
-        <v>11/10/2025, 3:18:26 PM</v>
+        <v>11/26/2025, 8:36:12 PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: prevent duplicate contexts and ensure base URL loads before tests
</commit_message>
<xml_diff>
--- a/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
+++ b/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
@@ -429,7 +429,7 @@
         <v>test.bulk.user1@brainstation-23.com</v>
       </c>
       <c r="D2" t="str">
-        <v>0b4b62a1-3e91-45cf-94ac-fb94a84ef9a4</v>
+        <v>3a87b84e-ad73-47ce-a66e-85738f511b12</v>
       </c>
     </row>
     <row r="3">
@@ -443,7 +443,7 @@
         <v>test.bulk.user2@brainstation-23.com</v>
       </c>
       <c r="D3" t="str">
-        <v>984b1f58-9233-4ec0-a193-30417b5ac9bd</v>
+        <v>48013d34-c952-42f2-a7d5-12d70ab56c71</v>
       </c>
     </row>
     <row r="4">
@@ -457,7 +457,7 @@
         <v>test.bulk.user3@brainstation-23.com</v>
       </c>
       <c r="D4" t="str">
-        <v>23ed4a6a-2467-48e5-a217-bf69106e9463</v>
+        <v>33cbeaee-1d80-4176-8909-d9cc52bb113f</v>
       </c>
     </row>
     <row r="5">
@@ -471,7 +471,7 @@
         <v>test.bulk.user4@brainstation-23.com</v>
       </c>
       <c r="D5" t="str">
-        <v>e8fc1a8e-bb04-421c-9fda-a519919c51b9</v>
+        <v>cc3e80ae-d970-4a7a-be85-8ce8bef43e6b</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>Report Generated</v>
       </c>
       <c r="B6" t="str">
-        <v>11/26/2025, 8:36:12 PM</v>
+        <v>11/27/2025, 4:51:11 PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test error due to code change
</commit_message>
<xml_diff>
--- a/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
+++ b/test_data/UserManagementTestData/UserExcelReport/excelReport.xlsx
@@ -429,7 +429,7 @@
         <v>test.bulk.user1@brainstation-23.com</v>
       </c>
       <c r="D2" t="str">
-        <v>3a87b84e-ad73-47ce-a66e-85738f511b12</v>
+        <v>c1190f23-06e2-416e-9037-33ba1488fcb0</v>
       </c>
     </row>
     <row r="3">
@@ -443,7 +443,7 @@
         <v>test.bulk.user2@brainstation-23.com</v>
       </c>
       <c r="D3" t="str">
-        <v>48013d34-c952-42f2-a7d5-12d70ab56c71</v>
+        <v>96de7f7e-adeb-408a-8965-e9773ba383d3</v>
       </c>
     </row>
     <row r="4">
@@ -457,7 +457,7 @@
         <v>test.bulk.user3@brainstation-23.com</v>
       </c>
       <c r="D4" t="str">
-        <v>33cbeaee-1d80-4176-8909-d9cc52bb113f</v>
+        <v>ae7ca3c6-a9b7-4e48-b3d0-fa7d63423342</v>
       </c>
     </row>
     <row r="5">
@@ -471,7 +471,7 @@
         <v>test.bulk.user4@brainstation-23.com</v>
       </c>
       <c r="D5" t="str">
-        <v>cc3e80ae-d970-4a7a-be85-8ce8bef43e6b</v>
+        <v>8ab035fb-0b44-4073-853e-a2a93b39e331</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>Report Generated</v>
       </c>
       <c r="B6" t="str">
-        <v>11/27/2025, 4:51:11 PM</v>
+        <v>11/27/2025, 6:20:32 PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>